<commit_message>
add -- last commit before fiasco
</commit_message>
<xml_diff>
--- a/uploads/forms-d9.XLSX
+++ b/uploads/forms-d9.XLSX
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -1200,8 +1200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1308,7 +1308,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>103</v>
@@ -1388,7 +1388,7 @@
         <v>16</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>103</v>
@@ -1408,7 +1408,7 @@
         <v>17</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>262</v>
+        <v>103</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>103</v>
@@ -1428,7 +1428,7 @@
         <v>11</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>262</v>
+        <v>103</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>103</v>
@@ -1448,7 +1448,7 @@
         <v>18</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>262</v>
+        <v>103</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>103</v>
@@ -1468,7 +1468,7 @@
         <v>104</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>262</v>
+        <v>103</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>103</v>
@@ -1488,7 +1488,7 @@
         <v>21</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>262</v>
+        <v>103</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>103</v>
@@ -1508,7 +1508,7 @@
         <v>19</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>262</v>
+        <v>103</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>103</v>
@@ -1528,7 +1528,7 @@
         <v>22</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>262</v>
+        <v>103</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>103</v>
@@ -1548,7 +1548,7 @@
         <v>23</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>262</v>
+        <v>103</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>103</v>
@@ -1568,7 +1568,7 @@
         <v>15</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>263</v>
+        <v>103</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>103</v>
@@ -1588,7 +1588,7 @@
         <v>13</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>263</v>
+        <v>103</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>103</v>
@@ -1608,7 +1608,7 @@
         <v>14</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>262</v>
+        <v>103</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>103</v>
@@ -1628,7 +1628,7 @@
         <v>105</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>262</v>
+        <v>103</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>103</v>
@@ -1648,7 +1648,7 @@
         <v>20</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>262</v>
+        <v>103</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>103</v>
@@ -1688,7 +1688,7 @@
         <v>99</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>262</v>
+        <v>103</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>103</v>

</xml_diff>